<commit_message>
H index manual update
</commit_message>
<xml_diff>
--- a/images/___images_sizing.xlsx
+++ b/images/___images_sizing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richtap/git/slovenskivedci/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F7F222-E2C2-BB46-874F-C70D1FDCB204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4ED7789-51DE-6E40-903A-32C577B51471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7820" yWindow="1760" windowWidth="26740" windowHeight="15500" xr2:uid="{FBABA11E-B330-2F49-B6C1-0584A0817DCB}"/>
   </bookViews>
@@ -94,12 +94,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -119,7 +117,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -407,7 +405,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -418,7 +416,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -429,30 +427,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" s="5" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
-        <v>2521</v>
-      </c>
-      <c r="B3" s="4">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>585</v>
+      </c>
+      <c r="B3" s="3">
         <f>A3/1.78</f>
-        <v>1416.2921348314605</v>
-      </c>
-      <c r="E3" s="5" t="s">
+        <v>328.65168539325845</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="5" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A4" s="5">
+    <row r="4" spans="1:5" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
         <f>B4*A9</f>
         <v>1406.2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>790</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Peter Molnar = Norsko
</commit_message>
<xml_diff>
--- a/images/___images_sizing.xlsx
+++ b/images/___images_sizing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richtap/git/slovenskivedci/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96383CB-75B6-3045-8EA8-65B544A0E3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D570D44B-036B-C148-AE99-010B5671EEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7820" yWindow="1760" windowWidth="26740" windowHeight="15500" xr2:uid="{FBABA11E-B330-2F49-B6C1-0584A0817DCB}"/>
   </bookViews>
@@ -439,11 +439,11 @@
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>1000</v>
+        <v>400</v>
       </c>
       <c r="B3" s="3">
         <f>A3/1.78</f>
-        <v>561.79775280898878</v>
+        <v>224.71910112359549</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>1</v>

</xml_diff>